<commit_message>
Listados listos del 16 de agosto
</commit_message>
<xml_diff>
--- a/Agosto/19 agosto/milpa alta/PLANTILLA LISTA DE ASPIRANTES_ITMA.xlsx
+++ b/Agosto/19 agosto/milpa alta/PLANTILLA LISTA DE ASPIRANTES_ITMA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27813"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITMA91\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proyecto01TICs\Documents\Evaluatec2024\Agosto\19 agosto\milpa alta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{7A1FF73C-4F99-4EB7-B0A7-60F77BC83F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2957A5D4-C9F7-4879-BAE4-879C86E1203B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1F054D-81C9-479F-82D9-01F2E3EAF445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D610CFFB-2790-104B-A52B-2B33694C28D9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{D610CFFB-2790-104B-A52B-2B33694C28D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
   <si>
     <t>INDICAR SI EL ASPIRANTE DEBE PRESENTARSE EN EL PLANTEL PARA REALIZAR EL EXAMEN</t>
   </si>
@@ -119,9 +119,6 @@
     <t>miryjisa23@gmail.com</t>
   </si>
   <si>
-    <t>IGEM-2009-202</t>
-  </si>
-  <si>
     <t>Olvera de la Cruz Nancy Paola</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>npoc.1998@gmail.com</t>
   </si>
   <si>
-    <t>IGEM-2009-203</t>
-  </si>
-  <si>
     <t>Ejemplo versión basica</t>
   </si>
   <si>
@@ -161,9 +155,6 @@
     <t>denis.rodri.sil@gmail.com</t>
   </si>
   <si>
-    <t>IBQ-2010-208</t>
-  </si>
-  <si>
     <t>Vargas Tellez Melanie Itzel</t>
   </si>
   <si>
@@ -203,9 +194,6 @@
     <t>moraneduardo.moran@gmail.com</t>
   </si>
   <si>
-    <t>ISIC-2010-225</t>
-  </si>
-  <si>
     <t>José Manuel Mendoza Rasgado</t>
   </si>
   <si>
@@ -215,9 +203,6 @@
     <t>mendozarasgadojosemanuel@gmail.com</t>
   </si>
   <si>
-    <t>ISIC-2010-226</t>
-  </si>
-  <si>
     <t>Esteva Lorenzo Leonardo Javier </t>
   </si>
   <si>
@@ -227,9 +212,6 @@
     <t>leonardo.javier.esteva.l.ce49@gmail.com</t>
   </si>
   <si>
-    <t>ISIC-2010-227</t>
-  </si>
-  <si>
     <t>Miroslava Baltazar Escamilla</t>
   </si>
   <si>
@@ -239,9 +221,6 @@
     <t xml:space="preserve">mirozhibaes@gmail.com </t>
   </si>
   <si>
-    <t>ISIC-2010-228</t>
-  </si>
-  <si>
     <t xml:space="preserve">Agustin Arenas Vázquez </t>
   </si>
   <si>
@@ -251,14 +230,14 @@
     <t>agustinarenasvazquez2006@gmail.com</t>
   </si>
   <si>
-    <t>ISIC-2010-229</t>
+    <t>2024/08/19 09:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -402,7 +381,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -415,9 +394,6 @@
     </xf>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -441,10 +417,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -462,23 +442,23 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="164" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="164" formatCode="h:mm\ AM/PM"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="hh:mm\ AM/PM"/>
+      <numFmt numFmtId="165" formatCode="hh:mm\ AM/PM"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="164" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+      <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -496,6 +476,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5925BC7A-0E73-734D-A0C9-B8A68F88FF64}" name="Tabla2" displayName="Tabla2" ref="A4:M16" totalsRowShown="0">
   <autoFilter ref="A4:M16" xr:uid="{5925BC7A-0E73-734D-A0C9-B8A68F88FF64}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:M16">
+    <sortCondition ref="F4:F16"/>
+  </sortState>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{F5111305-CA2B-DF41-BA05-5C9A177B7523}" name="FICHA"/>
     <tableColumn id="2" xr3:uid="{D956ADB6-2882-CB4B-9C6B-032AC358A5C1}" name="NOMBRE ASPIRANTE"/>
@@ -516,9 +499,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -556,7 +539,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -662,7 +645,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -804,7 +787,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -814,18 +797,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D137AA-41E5-5140-AC23-8A814C9A306A}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5" customWidth="1"/>
     <col min="2" max="2" width="27.75" customWidth="1"/>
     <col min="3" max="3" width="21.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.75" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.625" customWidth="1"/>
+    <col min="6" max="6" width="45.875" customWidth="1"/>
     <col min="7" max="7" width="13.75" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="16.125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.375" bestFit="1" customWidth="1"/>
@@ -834,28 +817,31 @@
     <col min="13" max="13" width="19.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="41.1" customHeight="1">
-      <c r="L1" s="24" t="s">
+    <row r="1" spans="1:15" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="25" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="21" customHeight="1" thickBot="1">
-      <c r="C2" s="22" t="s">
+    <row r="2" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="L2" s="24"/>
-    </row>
-    <row r="3" spans="1:15" ht="16.5" thickTop="1">
-      <c r="L3" s="24"/>
-    </row>
-    <row r="4" spans="1:15" ht="31.5">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="L2" s="25"/>
+    </row>
+    <row r="3" spans="1:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="25"/>
+    </row>
+    <row r="4" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -896,30 +882,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
+        <v>40</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>41</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
       </c>
       <c r="H5" s="2">
-        <v>45461</v>
+        <v>45466</v>
       </c>
       <c r="I5" s="3">
         <v>0.375</v>
@@ -936,35 +922,35 @@
       <c r="M5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="23" t="s">
+      <c r="N5" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="23"/>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="O5" s="24"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
         <v>20</v>
       </c>
       <c r="H6" s="2">
-        <v>45462</v>
+        <v>45464</v>
       </c>
       <c r="I6" s="3">
         <v>0.375</v>
@@ -982,30 +968,30 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>30</v>
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="2">
-        <v>45463</v>
+        <v>45465</v>
       </c>
       <c r="I7" s="3">
         <v>0.375</v>
@@ -1022,35 +1008,35 @@
       <c r="M7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N7" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O7" s="23"/>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="N7" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="24"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>35</v>
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s">
         <v>20</v>
       </c>
       <c r="H8" s="2">
-        <v>45464</v>
+        <v>45461</v>
       </c>
       <c r="I8" s="3">
         <v>0.375</v>
@@ -1068,30 +1054,30 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>39</v>
+        <v>2</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
         <v>20</v>
       </c>
       <c r="H9" s="2">
-        <v>45465</v>
+        <v>45462</v>
       </c>
       <c r="I9" s="3">
         <v>0.375</v>
@@ -1109,30 +1095,30 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>44</v>
+        <v>3</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
         <v>20</v>
       </c>
       <c r="H10" s="2">
-        <v>45466</v>
+        <v>45463</v>
       </c>
       <c r="I10" s="3">
         <v>0.375</v>
@@ -1150,24 +1136,24 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="F11" t="s">
         <v>48</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" t="s">
-        <v>51</v>
       </c>
       <c r="G11" t="s">
         <v>20</v>
@@ -1191,24 +1177,24 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>54</v>
+      <c r="B12" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>51</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G12" t="s">
         <v>20</v>
@@ -1232,24 +1218,24 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>58</v>
+      <c r="B13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G13" t="s">
         <v>20</v>
@@ -1273,24 +1259,24 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>62</v>
+      <c r="B14" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>57</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G14" t="s">
         <v>20</v>
@@ -1314,24 +1300,24 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>64</v>
+      <c r="B15" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>66</v>
+        <v>59</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>60</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G15" t="s">
         <v>20</v>
@@ -1355,24 +1341,24 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>70</v>
+        <v>61</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G16" t="s">
         <v>20</v>
@@ -1407,8 +1393,8 @@
   <hyperlinks>
     <hyperlink ref="D15" r:id="rId1" xr:uid="{EF28257B-1C78-4660-9EF4-90D2510F8412}"/>
     <hyperlink ref="D12" r:id="rId2" xr:uid="{6457E65E-1447-4B17-AE0D-EB0725B29225}"/>
-    <hyperlink ref="D9" r:id="rId3" xr:uid="{515113A4-2D2E-43B2-BDAD-C344AF983E0D}"/>
-    <hyperlink ref="D7" r:id="rId4" xr:uid="{77D74D00-0257-4CBA-B095-2AD6FFE29623}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{515113A4-2D2E-43B2-BDAD-C344AF983E0D}"/>
+    <hyperlink ref="D10" r:id="rId4" xr:uid="{77D74D00-0257-4CBA-B095-2AD6FFE29623}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>

</xml_diff>